<commit_message>
46th Commit Changed magic string class name and excel corrected
</commit_message>
<xml_diff>
--- a/docs/G89.2022.G04.FP.xlsx
+++ b/docs/G89.2022.G04.FP.xlsx
@@ -1,14 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\PycharmProjects\G89.2022.T04.FP\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899A4792-9538-4D4D-BD03-093757172CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="197" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="ECBV M1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="ECBV M2" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="SA M2" sheetId="3" r:id="rId6"/>
+    <sheet name="ECBV M1" sheetId="1" r:id="rId1"/>
+    <sheet name="ECBV M2" sheetId="2" r:id="rId2"/>
+    <sheet name="SA M2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1560,36 +1569,36 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="0"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="0"/>
       <name val="Arial"/>
     </font>
@@ -1599,7 +1608,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1621,88 +1630,85 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1892,34 +1898,39 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="3.38"/>
-    <col customWidth="1" min="2" max="2" width="8.38"/>
-    <col customWidth="1" min="3" max="3" width="12.13"/>
-    <col customWidth="1" min="4" max="4" width="7.13"/>
-    <col customWidth="1" min="5" max="5" width="14.75"/>
-    <col customWidth="1" min="6" max="6" width="36.88"/>
-    <col customWidth="1" min="7" max="7" width="59.38"/>
-    <col customWidth="1" min="8" max="8" width="74.25"/>
-    <col customWidth="1" min="9" max="9" width="13.38"/>
-    <col customWidth="1" min="10" max="10" width="17.13"/>
-    <col customWidth="1" min="11" max="11" width="66.63"/>
-    <col customWidth="1" min="12" max="12" width="32.38"/>
+    <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="68.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="84.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="76.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1957,9 +1968,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>12</v>
@@ -1995,9 +2006,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>12</v>
@@ -2033,9 +2044,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>12</v>
@@ -2071,9 +2082,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>12</v>
@@ -2109,9 +2120,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>12</v>
@@ -2147,9 +2158,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>12</v>
@@ -2185,9 +2196,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>12</v>
@@ -2223,9 +2234,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>12</v>
@@ -2261,9 +2272,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>12</v>
@@ -2299,9 +2310,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>12</v>
@@ -2337,9 +2348,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>12</v>
@@ -2375,9 +2386,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>12</v>
@@ -2413,9 +2424,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>12</v>
@@ -2451,9 +2462,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>12</v>
@@ -2489,9 +2500,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>12</v>
@@ -2527,9 +2538,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>12</v>
@@ -2565,9 +2576,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>12</v>
@@ -2603,9 +2614,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>12</v>
@@ -2641,9 +2652,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>12</v>
@@ -2679,9 +2690,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>12</v>
@@ -2717,9 +2728,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>12</v>
@@ -2755,9 +2766,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>12</v>
@@ -2793,9 +2804,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>12</v>
@@ -2831,9 +2842,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>12</v>
@@ -2869,9 +2880,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>12</v>
@@ -2907,9 +2918,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>12</v>
@@ -2936,7 +2947,7 @@
         <v>18</v>
       </c>
       <c r="J27" s="7">
-        <v>2.0221201E7</v>
+        <v>20221201</v>
       </c>
       <c r="K27" s="7" t="s">
         <v>34</v>
@@ -2945,9 +2956,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>12</v>
@@ -2984,38 +2995,41 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="3.25"/>
-    <col customWidth="1" min="2" max="2" width="13.25"/>
-    <col customWidth="1" min="3" max="3" width="13.13"/>
-    <col customWidth="1" min="4" max="4" width="16.13"/>
-    <col customWidth="1" min="5" max="5" width="15.25"/>
-    <col customWidth="1" min="6" max="6" width="26.25"/>
-    <col customWidth="1" min="7" max="7" width="52.38"/>
-    <col customWidth="1" min="8" max="8" width="74.38"/>
-    <col customWidth="1" min="9" max="9" width="67.13"/>
-    <col customWidth="1" min="10" max="10" width="20.88"/>
-    <col customWidth="1" min="11" max="11" width="101.88"/>
-    <col customWidth="1" min="12" max="12" width="66.75"/>
-    <col customWidth="1" min="13" max="13" width="63.13"/>
-    <col customWidth="1" min="14" max="14" width="14.5"/>
-    <col customWidth="1" min="15" max="15" width="23.63"/>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="85.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="76.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="122" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="75.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="73" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" customWidth="1"/>
+    <col min="15" max="15" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3056,9 +3070,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>12</v>
@@ -3097,9 +3111,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>12</v>
@@ -3138,9 +3152,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>12</v>
@@ -3179,9 +3193,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>12</v>
@@ -3220,9 +3234,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>12</v>
@@ -3261,9 +3275,9 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>12</v>
@@ -3302,9 +3316,9 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>12</v>
@@ -3343,9 +3357,9 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>12</v>
@@ -3384,9 +3398,9 @@
         <v>134</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>12</v>
@@ -3425,9 +3439,9 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>12</v>
@@ -3466,9 +3480,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>12</v>
@@ -3507,9 +3521,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>12</v>
@@ -3548,9 +3562,9 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>12</v>
@@ -3577,7 +3591,7 @@
         <v>109</v>
       </c>
       <c r="J14" s="11">
-        <v>123456.0</v>
+        <v>123456</v>
       </c>
       <c r="K14" s="11" t="s">
         <v>103</v>
@@ -3589,9 +3603,9 @@
         <v>160</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>12</v>
@@ -3630,9 +3644,9 @@
         <v>166</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>12</v>
@@ -3671,9 +3685,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>12</v>
@@ -3712,9 +3726,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>12</v>
@@ -3753,9 +3767,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>12</v>
@@ -3794,9 +3808,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>12</v>
@@ -3835,9 +3849,9 @@
         <v>166</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>12</v>
@@ -3867,7 +3881,7 @@
         <v>102</v>
       </c>
       <c r="K21" s="13">
-        <v>123.0</v>
+        <v>123</v>
       </c>
       <c r="L21" s="7" t="s">
         <v>190</v>
@@ -3877,33 +3891,36 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H102" sqref="H102"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="4.0"/>
-    <col customWidth="1" min="2" max="2" width="5.88"/>
-    <col customWidth="1" min="3" max="3" width="7.75"/>
-    <col customWidth="1" min="4" max="4" width="17.63"/>
-    <col customWidth="1" min="5" max="5" width="51.63"/>
-    <col customWidth="1" min="6" max="6" width="24.13"/>
-    <col customWidth="1" min="7" max="7" width="32.25"/>
-    <col customWidth="1" min="8" max="8" width="241.5"/>
-    <col customWidth="1" min="9" max="9" width="65.88"/>
-    <col customWidth="1" min="10" max="10" width="66.88"/>
+    <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="75.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="71.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -3935,12 +3952,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="7">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>198</v>
@@ -3965,12 +3982,12 @@
         <v>204</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="7">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>198</v>
@@ -3997,12 +4014,12 @@
         <v>209</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="11">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>198</v>
@@ -4029,12 +4046,12 @@
         <v>213</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="11">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>198</v>
@@ -4061,12 +4078,12 @@
         <v>217</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="7">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>198</v>
@@ -4093,12 +4110,12 @@
         <v>222</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="7">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>198</v>
@@ -4125,12 +4142,12 @@
         <v>226</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="11">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>198</v>
@@ -4157,12 +4174,12 @@
         <v>230</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="11">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>198</v>
@@ -4189,12 +4206,12 @@
         <v>234</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="7">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>235</v>
@@ -4221,12 +4238,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="11">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>235</v>
@@ -4253,12 +4270,12 @@
         <v>244</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="7">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>198</v>
@@ -4285,12 +4302,12 @@
         <v>248</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="7">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>198</v>
@@ -4317,12 +4334,12 @@
         <v>252</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="11">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>198</v>
@@ -4349,12 +4366,12 @@
         <v>256</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="17">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="11">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>198</v>
@@ -4381,12 +4398,12 @@
         <v>260</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="7">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>198</v>
@@ -4413,12 +4430,12 @@
         <v>264</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="7">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>198</v>
@@ -4445,12 +4462,12 @@
         <v>268</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="11">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>198</v>
@@ -4477,12 +4494,12 @@
         <v>256</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B19" s="11">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>198</v>
@@ -4509,12 +4526,12 @@
         <v>260</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B20" s="7">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>198</v>
@@ -4541,12 +4558,12 @@
         <v>276</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B21" s="7">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>198</v>
@@ -4573,12 +4590,12 @@
         <v>280</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B22" s="11">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>235</v>
@@ -4605,12 +4622,12 @@
         <v>284</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="B23" s="7">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>235</v>
@@ -4637,12 +4654,12 @@
         <v>284</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="B24" s="11">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>198</v>
@@ -4669,12 +4686,12 @@
         <v>290</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="B25" s="11">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>198</v>
@@ -4701,12 +4718,12 @@
         <v>294</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="B26" s="7">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>198</v>
@@ -4733,12 +4750,12 @@
         <v>298</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="B27" s="7">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>198</v>
@@ -4765,12 +4782,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="B28" s="11">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>198</v>
@@ -4797,12 +4814,12 @@
         <v>306</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="B29" s="11">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>198</v>
@@ -4829,12 +4846,12 @@
         <v>310</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="B30" s="7">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>198</v>
@@ -4861,12 +4878,12 @@
         <v>314</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="B31" s="7">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>198</v>
@@ -4893,12 +4910,12 @@
         <v>318</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="B32" s="11">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>198</v>
@@ -4925,12 +4942,12 @@
         <v>298</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="B33" s="11">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="C33" s="11" t="s">
         <v>198</v>
@@ -4957,12 +4974,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="B34" s="7">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>198</v>
@@ -4989,12 +5006,12 @@
         <v>326</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="B35" s="7">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>198</v>
@@ -5021,12 +5038,12 @@
         <v>330</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="B36" s="11">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>198</v>
@@ -5053,12 +5070,12 @@
         <v>334</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="B37" s="11">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="C37" s="11" t="s">
         <v>198</v>
@@ -5085,12 +5102,12 @@
         <v>338</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="B38" s="7">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>198</v>
@@ -5117,12 +5134,12 @@
         <v>298</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="B39" s="7">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>198</v>
@@ -5149,12 +5166,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="B40" s="11">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="C40" s="11" t="s">
         <v>198</v>
@@ -5181,12 +5198,12 @@
         <v>346</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="17">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="B41" s="11">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="C41" s="11" t="s">
         <v>198</v>
@@ -5213,12 +5230,12 @@
         <v>350</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="B42" s="7">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>235</v>
@@ -5245,12 +5262,12 @@
         <v>354</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="10">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="B43" s="11">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="C43" s="11" t="s">
         <v>235</v>
@@ -5277,12 +5294,12 @@
         <v>354</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="B44" s="7">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>235</v>
@@ -5309,12 +5326,12 @@
         <v>354</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="10">
-        <v>44.0</v>
+        <v>44</v>
       </c>
       <c r="B45" s="11">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>198</v>
@@ -5341,12 +5358,12 @@
         <v>362</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="10">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="B46" s="11">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>198</v>
@@ -5373,12 +5390,12 @@
         <v>366</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="B47" s="7">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>198</v>
@@ -5405,12 +5422,12 @@
         <v>371</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
-        <v>47.0</v>
+        <v>47</v>
       </c>
       <c r="B48" s="7">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>198</v>
@@ -5437,12 +5454,12 @@
         <v>375</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="17">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="B49" s="11">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="C49" s="11" t="s">
         <v>198</v>
@@ -5469,12 +5486,12 @@
         <v>362</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="10">
-        <v>49.0</v>
+        <v>49</v>
       </c>
       <c r="B50" s="11">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="C50" s="11" t="s">
         <v>198</v>
@@ -5501,12 +5518,12 @@
         <v>366</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="B51" s="7">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>198</v>
@@ -5533,12 +5550,12 @@
         <v>362</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
-        <v>51.0</v>
+        <v>51</v>
       </c>
       <c r="B52" s="7">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>198</v>
@@ -5565,12 +5582,12 @@
         <v>366</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="10">
-        <v>52.0</v>
+        <v>52</v>
       </c>
       <c r="B53" s="11">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="C53" s="11" t="s">
         <v>198</v>
@@ -5597,12 +5614,12 @@
         <v>387</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="17">
-        <v>53.0</v>
+        <v>53</v>
       </c>
       <c r="B54" s="11">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="C54" s="11" t="s">
         <v>198</v>
@@ -5629,12 +5646,12 @@
         <v>391</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="B55" s="7">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>198</v>
@@ -5661,12 +5678,12 @@
         <v>362</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
-        <v>55.0</v>
+        <v>55</v>
       </c>
       <c r="B56" s="7">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>198</v>
@@ -5693,12 +5710,12 @@
         <v>366</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="10">
-        <v>56.0</v>
+        <v>56</v>
       </c>
       <c r="B57" s="11">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="C57" s="11" t="s">
         <v>198</v>
@@ -5725,12 +5742,12 @@
         <v>362</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="10">
-        <v>57.0</v>
+        <v>57</v>
       </c>
       <c r="B58" s="11">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="C58" s="11" t="s">
         <v>198</v>
@@ -5757,12 +5774,12 @@
         <v>366</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
-        <v>58.0</v>
+        <v>58</v>
       </c>
       <c r="B59" s="7">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>198</v>
@@ -5789,12 +5806,12 @@
         <v>404</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
-        <v>59.0</v>
+        <v>59</v>
       </c>
       <c r="B60" s="7">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>198</v>
@@ -5821,12 +5838,12 @@
         <v>408</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="10">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="B61" s="11">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="C61" s="11" t="s">
         <v>198</v>
@@ -5853,12 +5870,12 @@
         <v>362</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="17">
-        <v>61.0</v>
+        <v>61</v>
       </c>
       <c r="B62" s="11">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="C62" s="11" t="s">
         <v>198</v>
@@ -5885,12 +5902,12 @@
         <v>366</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="6">
-        <v>62.0</v>
+        <v>62</v>
       </c>
       <c r="B63" s="7">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>198</v>
@@ -5917,12 +5934,12 @@
         <v>362</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="6">
-        <v>63.0</v>
+        <v>63</v>
       </c>
       <c r="B64" s="7">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="C64" s="7" t="s">
         <v>198</v>
@@ -5949,12 +5966,12 @@
         <v>366</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="10">
-        <v>64.0</v>
+        <v>64</v>
       </c>
       <c r="B65" s="11">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="C65" s="11" t="s">
         <v>198</v>
@@ -5981,12 +5998,12 @@
         <v>420</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="10">
-        <v>65.0</v>
+        <v>65</v>
       </c>
       <c r="B66" s="11">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="C66" s="11" t="s">
         <v>198</v>
@@ -6013,12 +6030,12 @@
         <v>424</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="15">
-        <v>66.0</v>
+        <v>66</v>
       </c>
       <c r="B67" s="7">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>198</v>
@@ -6045,12 +6062,12 @@
         <v>362</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
-        <v>67.0</v>
+        <v>67</v>
       </c>
       <c r="B68" s="7">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>198</v>
@@ -6077,12 +6094,12 @@
         <v>366</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="10">
-        <v>68.0</v>
+        <v>68</v>
       </c>
       <c r="B69" s="11">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="C69" s="11" t="s">
         <v>198</v>
@@ -6109,12 +6126,12 @@
         <v>362</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="10">
-        <v>69.0</v>
+        <v>69</v>
       </c>
       <c r="B70" s="11">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="C70" s="11" t="s">
         <v>198</v>
@@ -6141,12 +6158,12 @@
         <v>366</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="6">
-        <v>70.0</v>
+        <v>70</v>
       </c>
       <c r="B71" s="7">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>198</v>
@@ -6173,12 +6190,12 @@
         <v>437</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="6">
-        <v>71.0</v>
+        <v>71</v>
       </c>
       <c r="B72" s="7">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>198</v>
@@ -6205,12 +6222,12 @@
         <v>441</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="10">
-        <v>72.0</v>
+        <v>72</v>
       </c>
       <c r="B73" s="11">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="C73" s="11" t="s">
         <v>198</v>
@@ -6237,12 +6254,12 @@
         <v>362</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="10">
-        <v>73.0</v>
+        <v>73</v>
       </c>
       <c r="B74" s="11">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="C74" s="11" t="s">
         <v>198</v>
@@ -6269,12 +6286,12 @@
         <v>366</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="15">
-        <v>74.0</v>
+        <v>74</v>
       </c>
       <c r="B75" s="7">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="C75" s="7" t="s">
         <v>198</v>
@@ -6301,12 +6318,12 @@
         <v>362</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="6">
-        <v>75.0</v>
+        <v>75</v>
       </c>
       <c r="B76" s="7">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>198</v>
@@ -6333,12 +6350,12 @@
         <v>366</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="10">
-        <v>76.0</v>
+        <v>76</v>
       </c>
       <c r="B77" s="11">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="C77" s="11" t="s">
         <v>198</v>
@@ -6365,12 +6382,12 @@
         <v>453</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="10">
-        <v>77.0</v>
+        <v>77</v>
       </c>
       <c r="B78" s="11">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="C78" s="11" t="s">
         <v>198</v>
@@ -6397,12 +6414,12 @@
         <v>457</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="6">
-        <v>78.0</v>
+        <v>78</v>
       </c>
       <c r="B79" s="7">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>198</v>
@@ -6429,12 +6446,12 @@
         <v>362</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="15">
-        <v>79.0</v>
+        <v>79</v>
       </c>
       <c r="B80" s="7">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>198</v>
@@ -6461,12 +6478,12 @@
         <v>366</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="10">
-        <v>80.0</v>
+        <v>80</v>
       </c>
       <c r="B81" s="11">
-        <v>44.0</v>
+        <v>44</v>
       </c>
       <c r="C81" s="11" t="s">
         <v>235</v>
@@ -6493,12 +6510,12 @@
         <v>465</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="6">
-        <v>81.0</v>
+        <v>81</v>
       </c>
       <c r="B82" s="7">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="C82" s="7" t="s">
         <v>235</v>
@@ -6525,12 +6542,12 @@
         <v>468</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="10">
-        <v>82.0</v>
+        <v>82</v>
       </c>
       <c r="B83" s="11">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="C83" s="11" t="s">
         <v>235</v>
@@ -6557,12 +6574,12 @@
         <v>465</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="6">
-        <v>83.0</v>
+        <v>83</v>
       </c>
       <c r="B84" s="7">
-        <v>47.0</v>
+        <v>47</v>
       </c>
       <c r="C84" s="7" t="s">
         <v>235</v>
@@ -6589,12 +6606,12 @@
         <v>465</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="10">
-        <v>84.0</v>
+        <v>84</v>
       </c>
       <c r="B85" s="11">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="C85" s="11" t="s">
         <v>235</v>
@@ -6621,12 +6638,12 @@
         <v>476</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="6">
-        <v>85.0</v>
+        <v>85</v>
       </c>
       <c r="B86" s="7">
-        <v>49.0</v>
+        <v>49</v>
       </c>
       <c r="C86" s="7" t="s">
         <v>235</v>
@@ -6653,12 +6670,12 @@
         <v>465</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="10">
-        <v>86.0</v>
+        <v>86</v>
       </c>
       <c r="B87" s="11">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="C87" s="11" t="s">
         <v>235</v>
@@ -6685,12 +6702,12 @@
         <v>465</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="15">
-        <v>87.0</v>
+        <v>87</v>
       </c>
       <c r="B88" s="7">
-        <v>51.0</v>
+        <v>51</v>
       </c>
       <c r="C88" s="7" t="s">
         <v>235</v>
@@ -6717,12 +6734,12 @@
         <v>483</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="10">
-        <v>88.0</v>
+        <v>88</v>
       </c>
       <c r="B89" s="11">
-        <v>52.0</v>
+        <v>52</v>
       </c>
       <c r="C89" s="11" t="s">
         <v>235</v>
@@ -6749,12 +6766,12 @@
         <v>465</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="6">
-        <v>89.0</v>
+        <v>89</v>
       </c>
       <c r="B90" s="7">
-        <v>53.0</v>
+        <v>53</v>
       </c>
       <c r="C90" s="7" t="s">
         <v>235</v>
@@ -6781,12 +6798,12 @@
         <v>465</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="10">
-        <v>90.0</v>
+        <v>90</v>
       </c>
       <c r="B91" s="11">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="C91" s="11" t="s">
         <v>235</v>
@@ -6813,12 +6830,12 @@
         <v>491</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="6">
-        <v>91.0</v>
+        <v>91</v>
       </c>
       <c r="B92" s="7">
-        <v>55.0</v>
+        <v>55</v>
       </c>
       <c r="C92" s="7" t="s">
         <v>235</v>
@@ -6845,12 +6862,12 @@
         <v>465</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="17">
-        <v>92.0</v>
+        <v>92</v>
       </c>
       <c r="B93" s="11">
-        <v>56.0</v>
+        <v>56</v>
       </c>
       <c r="C93" s="11" t="s">
         <v>235</v>
@@ -6877,12 +6894,12 @@
         <v>465</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="6">
-        <v>93.0</v>
+        <v>93</v>
       </c>
       <c r="B94" s="7">
-        <v>57.0</v>
+        <v>57</v>
       </c>
       <c r="C94" s="7" t="s">
         <v>235</v>
@@ -6909,12 +6926,12 @@
         <v>498</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="10">
-        <v>94.0</v>
+        <v>94</v>
       </c>
       <c r="B95" s="11">
-        <v>58.0</v>
+        <v>58</v>
       </c>
       <c r="C95" s="11" t="s">
         <v>235</v>
@@ -6941,12 +6958,12 @@
         <v>465</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="6">
-        <v>95.0</v>
+        <v>95</v>
       </c>
       <c r="B96" s="7">
-        <v>59.0</v>
+        <v>59</v>
       </c>
       <c r="C96" s="7" t="s">
         <v>235</v>
@@ -6973,12 +6990,12 @@
         <v>465</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="10">
-        <v>96.0</v>
+        <v>96</v>
       </c>
       <c r="B97" s="11">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="C97" s="11" t="s">
         <v>235</v>
@@ -7005,12 +7022,12 @@
         <v>506</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="6">
-        <v>97.0</v>
+        <v>97</v>
       </c>
       <c r="B98" s="7">
-        <v>61.0</v>
+        <v>61</v>
       </c>
       <c r="C98" s="7" t="s">
         <v>235</v>
@@ -7037,9 +7054,9 @@
         <v>465</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="6">
-        <v>98.0</v>
+        <v>98</v>
       </c>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
@@ -7064,6 +7081,6 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>